<commit_message>
update README for english version
</commit_message>
<xml_diff>
--- a/example/TSNN/牛牛接口说明.xlsx
+++ b/example/TSNN/牛牛接口说明.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F996FDEE-AD2C-4B8D-951A-CEA0FE6971C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA6F1E6-7919-4D2E-8309-59A13A1658BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="变动历史" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="286">
   <si>
     <t>method</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1063,6 +1063,43 @@
   </si>
   <si>
     <t>戚鹏飞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nonce</t>
+  </si>
+  <si>
+    <t>u65</t>
+  </si>
+  <si>
+    <t>u66</t>
+  </si>
+  <si>
+    <t>对局轮次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随机数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getResult</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取对局结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i16[]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对局结果</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1386,6 +1423,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1393,15 +1439,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1714,7 +1751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74AC985B-4196-4B7D-B9B9-D16B1317C1E4}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -1747,10 +1784,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="50">
+      <c r="A3" s="53">
         <v>43349</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="42" t="s">
@@ -1764,8 +1801,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="51"/>
-      <c r="B4" s="54"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="50"/>
       <c r="C4" s="6" t="s">
         <v>97</v>
       </c>
@@ -1773,8 +1810,8 @@
       <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="51"/>
-      <c r="B5" s="54"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="6" t="s">
         <v>160</v>
       </c>
@@ -1782,8 +1819,8 @@
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="55"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="43" t="s">
         <v>161</v>
       </c>
@@ -1791,10 +1828,10 @@
       <c r="E6" s="61"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="52" t="s">
         <v>207</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="52" t="s">
         <v>208</v>
       </c>
       <c r="C7" t="s">
@@ -1803,7 +1840,7 @@
       <c r="D7" t="s">
         <v>209</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="E7" s="52" t="s">
         <v>210</v>
       </c>
     </row>
@@ -1819,104 +1856,104 @@
       <c r="E8" s="62"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="52" t="s">
         <v>252</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="52" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="42" t="s">
         <v>216</v>
       </c>
-      <c r="D9" s="53" t="s">
+      <c r="D9" s="52" t="s">
         <v>259</v>
       </c>
-      <c r="E9" s="53" t="s">
+      <c r="E9" s="52" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="54"/>
-      <c r="B10" s="54"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="54"/>
-      <c r="B11" s="54"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="54"/>
-      <c r="B12" s="54"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="54"/>
-      <c r="B13" s="54"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="54"/>
-      <c r="B14" s="54"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="54"/>
-      <c r="B15" s="54"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="50"/>
       <c r="C15" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="54"/>
-      <c r="B16" s="54"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="54"/>
-      <c r="B17" s="54"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="50" t="s">
         <v>261</v>
       </c>
-      <c r="E17" s="54"/>
+      <c r="E17" s="50"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="55"/>
-      <c r="B18" s="55"/>
+      <c r="A18" s="51"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="47" t="s">
@@ -1936,120 +1973,120 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="50" t="s">
         <v>273</v>
       </c>
-      <c r="B20" s="54" t="s">
+      <c r="B20" s="50" t="s">
         <v>272</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D20" s="53" t="s">
+      <c r="D20" s="52" t="s">
         <v>274</v>
       </c>
-      <c r="E20" s="53" t="s">
+      <c r="E20" s="52" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="54"/>
-      <c r="B21" s="54"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="54"/>
-      <c r="B22" s="54"/>
+      <c r="A22" s="50"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="54"/>
-      <c r="B23" s="54"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="54"/>
-      <c r="B24" s="54"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="54"/>
-      <c r="B25" s="54"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="54"/>
-      <c r="B26" s="54"/>
+      <c r="A26" s="50"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="54"/>
-      <c r="B27" s="54"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="54"/>
-      <c r="B28" s="54"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="50"/>
       <c r="C28" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="54"/>
-      <c r="B29" s="54"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="50"/>
       <c r="C29" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="54"/>
-      <c r="B30" s="54"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="50"/>
       <c r="C30" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="55"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="51"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="43" t="s">
         <v>226</v>
       </c>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C32" s="6"/>
@@ -2059,6 +2096,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="E7:E8"/>
     <mergeCell ref="B20:B31"/>
     <mergeCell ref="A20:A31"/>
     <mergeCell ref="D20:D31"/>
@@ -2068,13 +2112,6 @@
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="B9:B18"/>
     <mergeCell ref="A9:A18"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2084,10 +2121,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M114"/>
+  <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4341,6 +4378,78 @@
       <c r="J114" s="16"/>
       <c r="K114" s="16"/>
       <c r="L114" s="46"/>
+    </row>
+    <row r="116" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A116" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="B116" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="C116" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D116" s="29"/>
+      <c r="E116" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F116" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G116" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H116" s="29"/>
+      <c r="I116" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="J116" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="K116" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="L116" s="29"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A117" s="21"/>
+      <c r="B117" s="20"/>
+      <c r="C117" s="20"/>
+      <c r="D117" s="29"/>
+      <c r="E117" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="F117" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="G117" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="H117" s="29"/>
+      <c r="I117" s="21"/>
+      <c r="J117" s="20"/>
+      <c r="K117" s="20"/>
+      <c r="L117" s="29"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A118" s="21"/>
+      <c r="B118" s="20"/>
+      <c r="C118" s="20"/>
+      <c r="D118" s="29"/>
+      <c r="E118" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="F118" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="G118" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="H118" s="29"/>
+      <c r="I118" s="21"/>
+      <c r="J118" s="20"/>
+      <c r="K118" s="20"/>
+      <c r="L118" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>